<commit_message>
Model validation work, added price surrogate, price based optimization
</commit_message>
<xml_diff>
--- a/COMPONENTS/Battery/BatteryDatabase.xlsx
+++ b/COMPONENTS/Battery/BatteryDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renkert2\Documents\ARG_Research\QuadrotorOptimization\COMPONENTS\Battery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701FF17C-75EE-44CF-A1AD-DB0DE625A630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D41DD05-BE5C-471C-8C4B-A1834BB3EFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EAB02434-AA89-48FD-AFF1-30E2F2364EC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
   <si>
     <t>Make</t>
   </si>
@@ -315,6 +315,15 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Pack Price</t>
   </si>
 </sst>
 </file>
@@ -678,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974502DF-30A3-446B-868F-1B65DF404E6A}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,15 +698,16 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -705,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -727,8 +737,11 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -750,8 +763,11 @@
       <c r="J3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -773,13 +789,16 @@
       <c r="J4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -793,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -824,8 +843,11 @@
       <c r="J7">
         <v>0.40500000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>56.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -856,8 +878,11 @@
       <c r="J8">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>42.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -888,8 +913,11 @@
       <c r="J9">
         <v>7.5999999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>21.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -920,8 +948,11 @@
       <c r="J10">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>27.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -952,8 +983,11 @@
       <c r="J11">
         <v>0.156</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -984,8 +1018,11 @@
       <c r="J12">
         <v>0.16200000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>22.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1016,8 +1053,11 @@
       <c r="J13">
         <v>0.52900000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>69.989999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1048,8 +1088,11 @@
       <c r="J14">
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>55.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1080,8 +1123,11 @@
       <c r="J15">
         <v>0.21199999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>26.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1112,8 +1158,11 @@
       <c r="J16">
         <v>0.13700000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1144,8 +1193,11 @@
       <c r="J17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>18.989999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1176,8 +1228,11 @@
       <c r="J18">
         <v>8.4000000000000005E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1208,8 +1263,11 @@
       <c r="J19">
         <v>4.2999999999999997E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1240,8 +1298,11 @@
       <c r="J20">
         <v>0.59799999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>82.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1272,8 +1333,11 @@
       <c r="J21">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>116.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1304,8 +1368,11 @@
       <c r="J22">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>65.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1336,8 +1403,11 @@
       <c r="J23">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>104.97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1368,8 +1438,11 @@
       <c r="J24">
         <v>0.21199999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1400,8 +1473,11 @@
       <c r="J25">
         <v>0.17299999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1432,8 +1508,11 @@
       <c r="J26">
         <v>0.14799999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>23.97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1464,8 +1543,11 @@
       <c r="J27">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>26.97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1496,8 +1578,11 @@
       <c r="J28">
         <v>0.249</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>31.99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1528,8 +1613,11 @@
       <c r="J29">
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>129.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1560,8 +1648,11 @@
       <c r="J30">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>81.99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1592,8 +1683,11 @@
       <c r="J31">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1624,8 +1718,11 @@
       <c r="J32">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>42.97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1656,8 +1753,11 @@
       <c r="J33">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>32.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1688,8 +1788,11 @@
       <c r="J34">
         <v>9.4E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1720,8 +1823,11 @@
       <c r="J35">
         <v>5.0999999999999997E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1752,8 +1858,11 @@
       <c r="J36">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1784,8 +1893,11 @@
       <c r="J37">
         <v>0.21199999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>29.99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1816,8 +1928,11 @@
       <c r="J38">
         <v>0.11600000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1847,6 +1962,9 @@
       </c>
       <c r="J39">
         <v>0.63</v>
+      </c>
+      <c r="K39">
+        <v>75.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>